<commit_message>
pushing again before branching just in case
</commit_message>
<xml_diff>
--- a/API docs/KeepAppAPI.xlsx
+++ b/API docs/KeepAppAPI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esad/Documents/KeepApp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esad/Workspace/keepapp-backend/API docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B3C569-C14F-B146-9379-ECDE0462EBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254EF594-33E5-B74F-BD17-5727F86FFE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{BEBEFC99-B4EA-C443-99A8-E6B575669E25}"/>
   </bookViews>
@@ -504,12 +504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -520,6 +514,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32B0303-0B35-044E-8C49-A625EDEF7F16}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1159,10 +1159,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="14"/>
       <c r="F3" s="15" t="s">
         <v>23</v>
       </c>
@@ -1173,107 +1173,107 @@
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>0</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <v>0</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="9">
         <v>2</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>1</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>3</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="11">
         <v>2</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="11">
         <v>4</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>3</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>4</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>23</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some api funcs implemented.
</commit_message>
<xml_diff>
--- a/API docs/KeepAppAPI.xlsx
+++ b/API docs/KeepAppAPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esad/Workspace/keepapp-backend/API docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541FC799-52FC-BD42-8A1F-411F2F598FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C894C4F3-10CA-7546-A65A-DFAAC9151584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{BEBEFC99-B4EA-C443-99A8-E6B575669E25}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
   <si>
     <t>METHOD</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Returns the rooms that user has access to. (Admin -&gt; all. Keeper -&gt; assigned.)</t>
   </si>
   <si>
-    <t>/message</t>
-  </si>
-  <si>
     <t>Sends new message.</t>
   </si>
   <si>
@@ -157,18 +154,8 @@
   </si>
   <si>
     <t>{
-  "message":{
-    "text":"AD123 numaralı odanın kapısı açılmıyor içeri giremedim."
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
   "success":1
 }</t>
-  </si>
-  <si>
-    <t>/user/login</t>
   </si>
   <si>
     <t>Creates JWT token and sends it to the client in a cookie.</t>
@@ -183,13 +170,7 @@
 }</t>
   </si>
   <si>
-    <t>/user/logout</t>
-  </si>
-  <si>
     <t>Destroys the JWT token and sends headers to the client to do the same</t>
-  </si>
-  <si>
-    <t>/user/register</t>
   </si>
   <si>
     <t>Creates new user.</t>
@@ -209,9 +190,6 @@
   </si>
   <si>
     <t>The behaviour of this function is currently wrong. Only the super admin can create an admin,  and an admin (logged in) should only be able to crate a keeper. In the next versions the userType parameter will be deprecated.</t>
-  </si>
-  <si>
-    <t>/message/{start}/{n}</t>
   </si>
   <si>
     <t>Returns {n} last messages starting from {start}.</t>
@@ -429,6 +407,176 @@
   ],
   "success": 1
 }</t>
+  </si>
+  <si>
+    <t>/keeperGroups</t>
+  </si>
+  <si>
+    <t>Returns every keeper group.</t>
+  </si>
+  <si>
+    <t>/keeperGroups/id</t>
+  </si>
+  <si>
+    <t>/keeperGroups/2</t>
+  </si>
+  <si>
+    <t>Creates new keeper group.</t>
+  </si>
+  <si>
+    <t>Data in body.</t>
+  </si>
+  <si>
+    <t>{
+  "name": "Kat1",
+  "rooms": ["VK500", "VK501", "VK502"]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "id": 3,
+  "success":1
+}</t>
+  </si>
+  <si>
+    <t>{
+  "keeperGroups": [
+    {
+      "id": 1,
+      "name": "Kat1",
+      "rooms": ["VK501", "VK502"],
+      "keeperIds":[1,2,3,9]
+    },
+    {
+      "id": 2,
+      "name": "Kat2",
+      "rooms": ["VK601", "VK602"],
+      "keeperIds":[1,2,4,5]
+    }
+  ],
+  "success": 1
+}</t>
+  </si>
+  <si>
+    <t>{
+  "keeperGroup": {
+    "id": 2,
+    "name": "Kat2",
+    "rooms": ["VK701"],
+    "keeperIds": [1, 2, 4, 5]
+  },
+  "success": 1
+}</t>
+  </si>
+  <si>
+    <t>/users/login</t>
+  </si>
+  <si>
+    <t>/users/logout</t>
+  </si>
+  <si>
+    <t>/users/register</t>
+  </si>
+  <si>
+    <t>/users/{id}</t>
+  </si>
+  <si>
+    <t>{
+  "password": "hunter2"
+  ||
+  "keeperGroupIds": [1,3,5]
+}</t>
+  </si>
+  <si>
+    <t>Returns keeper group with given id.</t>
+  </si>
+  <si>
+    <t>Updates user data. Only the password and keeper groups can be updated. If the user with given id is not a keeper, the user won't be assigned keeper groups.</t>
+  </si>
+  <si>
+    <t>Id in url, password or keeperGroupIds in body.</t>
+  </si>
+  <si>
+    <t>This function will remove keeper from the groups he/she is in and will assing him/her to given groups so that the removal or addition to groups can be done in a single call. To retrieve the groups user is assigned to see GET /users/{id}.</t>
+  </si>
+  <si>
+    <t>Id in the url.</t>
+  </si>
+  <si>
+    <t>Retrieves user data for admin or keeper accounts</t>
+  </si>
+  <si>
+    <t>{
+    "id": 1,
+    "username": "esad",
+    "userType": 2,
+    "keeperGroups": [
+        {
+            "id": 1,
+            "name": "group A",
+            "rooms": [
+                "room 102",
+                "VK510"
+            ],
+            "keeperIds": [
+                1,
+                2
+            ]
+        }
+    ],
+    "records": [{
+            "id": 14,
+            "roomId": 13,
+            "time": "2022-02-08 16:56:09.139746",
+            "keeperId": 5,
+            "checkList": {
+                "yatak": 3,
+                "televizyon": 2,
+                "kettle": 4
+            },
+            "notes": "Misafir yatağa sıçmış.",
+            "photos": [
+                "example.com/example.jpg",
+                "example.com/example2.jpg"
+            ]
+        }],
+    "messages": [
+        {
+            "id": 1,
+            "senderId": 1,
+            "time": "2022-01-26 12:26:28.798261",
+            "message": "hey wassup",
+            "is_read": false
+        },
+        {
+            "id": 2,
+            "senderId": 1,
+            "time": "2022-01-26 14:27:07.468491",
+            "message": "heyyo bosss",
+            "is_read": false
+        }
+    ],
+    "success": 1
+}</t>
+  </si>
+  <si>
+    <t>{    "text":"AD123 numaralı odanın kapısı açılmıyor içeri giremedim."
+}</t>
+  </si>
+  <si>
+    <t>/messages</t>
+  </si>
+  <si>
+    <t>/messages/{start}/{n}</t>
+  </si>
+  <si>
+    <t>/messages/{id}</t>
+  </si>
+  <si>
+    <t>Updates is_read field of message with given id.</t>
+  </si>
+  <si>
+    <t>/message/1</t>
   </si>
 </sst>
 </file>
@@ -914,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32B0303-0B35-044E-8C49-A625EDEF7F16}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="108" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,7 +1073,7 @@
     <col min="1" max="1" width="9.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
@@ -952,10 +1100,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="5" customFormat="1" ht="255" x14ac:dyDescent="0.2">
@@ -963,7 +1111,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>31</v>
@@ -978,7 +1126,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="204" x14ac:dyDescent="0.2">
@@ -989,7 +1137,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -998,10 +1146,10 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="153" x14ac:dyDescent="0.2">
@@ -1009,25 +1157,25 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="340" x14ac:dyDescent="0.2">
@@ -1035,22 +1183,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="255" x14ac:dyDescent="0.2">
@@ -1058,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>29</v>
@@ -1067,13 +1215,13 @@
         <v>30</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="153" x14ac:dyDescent="0.2">
@@ -1081,19 +1229,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="404" x14ac:dyDescent="0.2">
@@ -1101,16 +1252,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="204" x14ac:dyDescent="0.2">
@@ -1118,79 +1269,88 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>36</v>
+      <c r="H12" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" ht="372" x14ac:dyDescent="0.2">
@@ -1198,91 +1358,227 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="241" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="E17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" ht="187" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="B19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="356" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>65</v>
+      <c r="B22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API funcs. finished (there might be som things I forgot about), jwt refresh implemented, wrote some todos and comments. Next up swagger documentation.
</commit_message>
<xml_diff>
--- a/API docs/KeepAppAPI.xlsx
+++ b/API docs/KeepAppAPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esad/Workspace/keepapp-backend/API docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C894C4F3-10CA-7546-A65A-DFAAC9151584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A351D401-23D6-A042-BBEB-CA34E1DC5251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{BEBEFC99-B4EA-C443-99A8-E6B575669E25}"/>
   </bookViews>
@@ -479,13 +479,6 @@
   </si>
   <si>
     <t>/users/{id}</t>
-  </si>
-  <si>
-    <t>{
-  "password": "hunter2"
-  ||
-  "keeperGroupIds": [1,3,5]
-}</t>
   </si>
   <si>
     <t>Returns keeper group with given id.</t>
@@ -577,6 +570,13 @@
   </si>
   <si>
     <t>/message/1</t>
+  </si>
+  <si>
+    <t>{ "oldPassword":"sa",
+  "newPassword": "hunter2"
+  ||
+  "keeperGroupIds": [1,3,5]
+}</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32B0303-0B35-044E-8C49-A625EDEF7F16}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="108" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="108" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1335,7 +1335,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>32</v>
@@ -1344,7 +1344,7 @@
         <v>33</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>34</v>
@@ -1358,7 +1358,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>44</v>
@@ -1381,16 +1381,16 @@
         <v>73</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>34</v>
@@ -1480,19 +1480,19 @@
         <v>96</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>58</v>
@@ -1506,13 +1506,13 @@
         <v>96</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>58</v>
@@ -1543,7 +1543,7 @@
         <v>85</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>

</xml_diff>